<commit_message>
fixed issues. Updated spreadsheet to include 'groups'
</commit_message>
<xml_diff>
--- a/public/assets/excel/test input spreadsheet.xlsx
+++ b/public/assets/excel/test input spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rory.webber\Documents\projects\arup-carbon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rory.webber\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D69A2B-5A85-443A-8CD4-179A9F490CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6544AF8B-CDDE-4DE7-B403-9BEB8254C90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14190" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{7CD4E38A-B91F-4A7D-9B2E-EAEA1E44909C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Material</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t>THIS IS A FAKE MATERIAL!!!!</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Cop</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -98,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,8 +132,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,17 +162,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -154,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,159 +485,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2459ACA3-BF4D-4B85-A3C6-27F827F5F09B}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>31</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>2800</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>0.39</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>1760</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>0.91</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>1440</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.04</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>2400</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>0.05</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="2">
         <v>7.4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>8940</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0.05</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>